<commit_message>
Added welcome mail generator
</commit_message>
<xml_diff>
--- a/empListReliance.xlsx
+++ b/empListReliance.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Rishabh</t>
   </si>
   <si>
-    <t xml:space="preserve">ridhabhthaney</t>
+    <t xml:space="preserve">ridhabhthaney@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Account 2</t>
@@ -160,15 +160,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.3962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,7 +185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -214,6 +214,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="ridhabhthaney@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>